<commit_message>
[Docker] - add Dockerfile and .dockerignore
</commit_message>
<xml_diff>
--- a/tools/text-wrapper/language_main.xlsx
+++ b/tools/text-wrapper/language_main.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyGame\Now\customer-delivery-food\tools\text-wrapper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C29BAFD-A61A-4D94-87DB-CF149C0EC9C7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67A6323B-FE2D-49C3-AE4E-64EBE6F357EE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$690</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$691</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Sheet1!$1:$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="383">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="402">
   <si>
     <t>EN</t>
   </si>
@@ -329,24 +329,6 @@
     <t>txt_restaurant_filter_3</t>
   </si>
   <si>
-    <t>Most discount</t>
-  </si>
-  <si>
-    <t>Near me</t>
-  </si>
-  <si>
-    <t>Giảm giá nhiều nhất</t>
-  </si>
-  <si>
-    <t>Mới nhất</t>
-  </si>
-  <si>
-    <t>Gần tôi</t>
-  </si>
-  <si>
-    <t>Latest</t>
-  </si>
-  <si>
     <t>txt_district</t>
   </si>
   <si>
@@ -1188,6 +1170,82 @@
   </si>
   <si>
     <t>Cancel</t>
+  </si>
+  <si>
+    <t>txt_collections</t>
+  </si>
+  <si>
+    <t>Collections</t>
+  </si>
+  <si>
+    <t>txt_view_all</t>
+  </si>
+  <si>
+    <t>Xem tất cả</t>
+  </si>
+  <si>
+    <t>txt_nearby</t>
+  </si>
+  <si>
+    <t>Gần đây</t>
+  </si>
+  <si>
+    <t>Nearby</t>
+  </si>
+  <si>
+    <t>txt_top_sales</t>
+  </si>
+  <si>
+    <t>Bán chạy</t>
+  </si>
+  <si>
+    <t>Top sales</t>
+  </si>
+  <si>
+    <t>txt_best_rated</t>
+  </si>
+  <si>
+    <t>Đánh giá</t>
+  </si>
+  <si>
+    <t>Best rated</t>
+  </si>
+  <si>
+    <t>txt_load_more</t>
+  </si>
+  <si>
+    <t>Xem thêm</t>
+  </si>
+  <si>
+    <t>Load more</t>
+  </si>
+  <si>
+    <t>Bộ sưu tập</t>
+  </si>
+  <si>
+    <t>txt_most_discount</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Giảm giá </t>
+  </si>
+  <si>
+    <t>Discount</t>
+  </si>
+  <si>
+    <t>txt_restaurant_filter_4</t>
+  </si>
+  <si>
+    <t>txt_require_address</t>
+  </si>
+  <si>
+    <t>Vui lòng định vị địa chỉ nhận hàng</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Please pick up the address</t>
+  </si>
+  <si>
+    <t>Đặt hàng</t>
   </si>
 </sst>
 </file>
@@ -1633,13 +1691,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:K1099"/>
+  <dimension ref="A1:K1100"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C102" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C134" sqref="C134"/>
+      <selection pane="bottomRight" activeCell="B118" sqref="B118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5"/>
@@ -1816,7 +1874,7 @@
         <v>22</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>23</v>
@@ -2241,7 +2299,7 @@
       </c>
       <c r="D31" s="3"/>
       <c r="E31" s="4"/>
-      <c r="F31" s="4"/>
+      <c r="F31" s="7"/>
       <c r="G31" s="4"/>
       <c r="H31" s="4"/>
       <c r="I31" s="4"/>
@@ -2260,7 +2318,7 @@
       </c>
       <c r="D32" s="3"/>
       <c r="E32" s="4"/>
-      <c r="F32" s="4"/>
+      <c r="F32" s="7"/>
       <c r="G32" s="4"/>
       <c r="H32" s="4"/>
       <c r="I32" s="4"/>
@@ -2279,7 +2337,7 @@
       </c>
       <c r="D33" s="3"/>
       <c r="E33" s="4"/>
-      <c r="F33" s="4"/>
+      <c r="F33" s="7"/>
       <c r="G33" s="4"/>
       <c r="H33" s="4"/>
       <c r="I33" s="4"/>
@@ -2291,14 +2349,14 @@
         <v>93</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>98</v>
+        <v>382</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>96</v>
+        <v>383</v>
       </c>
       <c r="D34" s="3"/>
       <c r="E34" s="4"/>
-      <c r="F34" s="4"/>
+      <c r="F34" s="7"/>
       <c r="G34" s="4"/>
       <c r="H34" s="4"/>
       <c r="I34" s="4"/>
@@ -2310,10 +2368,10 @@
         <v>94</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>99</v>
+        <v>385</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>101</v>
+        <v>386</v>
       </c>
       <c r="D35" s="3"/>
       <c r="E35" s="4"/>
@@ -2329,10 +2387,10 @@
         <v>95</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>100</v>
+        <v>388</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>97</v>
+        <v>389</v>
       </c>
       <c r="D36" s="3"/>
       <c r="E36" s="4"/>
@@ -2345,13 +2403,13 @@
     </row>
     <row r="37" spans="1:11" s="2" customFormat="1">
       <c r="A37" s="4" t="s">
-        <v>102</v>
+        <v>397</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>103</v>
+        <v>395</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>104</v>
+        <v>396</v>
       </c>
       <c r="D37" s="3"/>
       <c r="E37" s="4"/>
@@ -2364,13 +2422,13 @@
     </row>
     <row r="38" spans="1:11" s="2" customFormat="1">
       <c r="A38" s="4" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>337</v>
+        <v>97</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="D38" s="3"/>
       <c r="E38" s="4"/>
@@ -2383,13 +2441,13 @@
     </row>
     <row r="39" spans="1:11" s="2" customFormat="1">
       <c r="A39" s="4" t="s">
-        <v>222</v>
+        <v>99</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>107</v>
+        <v>331</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>119</v>
+        <v>100</v>
       </c>
       <c r="D39" s="3"/>
       <c r="E39" s="4"/>
@@ -2402,13 +2460,13 @@
     </row>
     <row r="40" spans="1:11" s="2" customFormat="1">
       <c r="A40" s="4" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="D40" s="3"/>
       <c r="E40" s="4"/>
@@ -2421,13 +2479,13 @@
     </row>
     <row r="41" spans="1:11" s="2" customFormat="1">
       <c r="A41" s="4" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="D41" s="3"/>
       <c r="E41" s="4"/>
@@ -2440,13 +2498,13 @@
     </row>
     <row r="42" spans="1:11" s="2" customFormat="1">
       <c r="A42" s="4" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="D42" s="3"/>
       <c r="E42" s="4"/>
@@ -2459,13 +2517,13 @@
     </row>
     <row r="43" spans="1:11" s="2" customFormat="1">
       <c r="A43" s="4" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="D43" s="3"/>
       <c r="E43" s="4"/>
@@ -2478,13 +2536,13 @@
     </row>
     <row r="44" spans="1:11" s="2" customFormat="1">
       <c r="A44" s="4" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="D44" s="3"/>
       <c r="E44" s="4"/>
@@ -2497,13 +2555,13 @@
     </row>
     <row r="45" spans="1:11" s="2" customFormat="1">
       <c r="A45" s="4" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="D45" s="3"/>
       <c r="E45" s="4"/>
@@ -2516,13 +2574,13 @@
     </row>
     <row r="46" spans="1:11" s="2" customFormat="1">
       <c r="A46" s="4" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="D46" s="3"/>
       <c r="E46" s="4"/>
@@ -2535,13 +2593,13 @@
     </row>
     <row r="47" spans="1:11" s="2" customFormat="1">
       <c r="A47" s="4" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="D47" s="3"/>
       <c r="E47" s="4"/>
@@ -2554,13 +2612,13 @@
     </row>
     <row r="48" spans="1:11" s="2" customFormat="1">
       <c r="A48" s="4" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="D48" s="3"/>
       <c r="E48" s="4"/>
@@ -2573,13 +2631,13 @@
     </row>
     <row r="49" spans="1:11" s="2" customFormat="1">
       <c r="A49" s="4" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="D49" s="3"/>
       <c r="E49" s="4"/>
@@ -2592,13 +2650,13 @@
     </row>
     <row r="50" spans="1:11" s="2" customFormat="1">
       <c r="A50" s="4" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="D50" s="3"/>
       <c r="E50" s="4"/>
@@ -2611,13 +2669,13 @@
     </row>
     <row r="51" spans="1:11" s="2" customFormat="1">
       <c r="A51" s="4" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>131</v>
+        <v>112</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>142</v>
+        <v>124</v>
       </c>
       <c r="D51" s="3"/>
       <c r="E51" s="4"/>
@@ -2630,13 +2688,13 @@
     </row>
     <row r="52" spans="1:11" s="2" customFormat="1">
       <c r="A52" s="4" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="D52" s="3"/>
       <c r="E52" s="4"/>
@@ -2649,13 +2707,13 @@
     </row>
     <row r="53" spans="1:11" s="2" customFormat="1">
       <c r="A53" s="4" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="D53" s="3"/>
       <c r="E53" s="4"/>
@@ -2668,13 +2726,13 @@
     </row>
     <row r="54" spans="1:11" s="2" customFormat="1">
       <c r="A54" s="4" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="D54" s="3"/>
       <c r="E54" s="4"/>
@@ -2687,13 +2745,13 @@
     </row>
     <row r="55" spans="1:11" s="2" customFormat="1">
       <c r="A55" s="4" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="D55" s="3"/>
       <c r="E55" s="4"/>
@@ -2706,13 +2764,13 @@
     </row>
     <row r="56" spans="1:11" s="2" customFormat="1">
       <c r="A56" s="4" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="D56" s="3"/>
       <c r="E56" s="4"/>
@@ -2725,13 +2783,13 @@
     </row>
     <row r="57" spans="1:11" s="2" customFormat="1">
       <c r="A57" s="4" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="D57" s="3"/>
       <c r="E57" s="4"/>
@@ -2744,13 +2802,13 @@
     </row>
     <row r="58" spans="1:11" s="2" customFormat="1">
       <c r="A58" s="4" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="D58" s="3"/>
       <c r="E58" s="4"/>
@@ -2763,13 +2821,13 @@
     </row>
     <row r="59" spans="1:11" s="2" customFormat="1">
       <c r="A59" s="4" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="D59" s="3"/>
       <c r="E59" s="4"/>
@@ -2782,13 +2840,13 @@
     </row>
     <row r="60" spans="1:11" s="2" customFormat="1">
       <c r="A60" s="4" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="D60" s="3"/>
       <c r="E60" s="4"/>
@@ -2801,13 +2859,13 @@
     </row>
     <row r="61" spans="1:11" s="2" customFormat="1">
       <c r="A61" s="4" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="B61" s="7" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="D61" s="3"/>
       <c r="E61" s="4"/>
@@ -2820,13 +2878,13 @@
     </row>
     <row r="62" spans="1:11" s="2" customFormat="1">
       <c r="A62" s="4" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="B62" s="7" t="s">
-        <v>172</v>
+        <v>135</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>173</v>
+        <v>146</v>
       </c>
       <c r="D62" s="3"/>
       <c r="E62" s="4"/>
@@ -2839,13 +2897,13 @@
     </row>
     <row r="63" spans="1:11" s="2" customFormat="1">
       <c r="A63" s="4" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>261</v>
+        <v>166</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>289</v>
+        <v>167</v>
       </c>
       <c r="D63" s="3"/>
       <c r="E63" s="4"/>
@@ -2858,13 +2916,13 @@
     </row>
     <row r="64" spans="1:11" s="2" customFormat="1">
       <c r="A64" s="4" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="B64" s="7" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>277</v>
+        <v>283</v>
       </c>
       <c r="D64" s="3"/>
       <c r="E64" s="4"/>
@@ -2877,13 +2935,13 @@
     </row>
     <row r="65" spans="1:11" s="2" customFormat="1">
       <c r="A65" s="4" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
       <c r="D65" s="3"/>
       <c r="E65" s="4"/>
@@ -2896,13 +2954,13 @@
     </row>
     <row r="66" spans="1:11" s="2" customFormat="1">
       <c r="A66" s="4" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="B66" s="7" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="D66" s="3"/>
       <c r="E66" s="4"/>
@@ -2915,13 +2973,13 @@
     </row>
     <row r="67" spans="1:11" s="2" customFormat="1">
       <c r="A67" s="4" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="B67" s="7" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="D67" s="3"/>
       <c r="E67" s="4"/>
@@ -2934,13 +2992,13 @@
     </row>
     <row r="68" spans="1:11" s="2" customFormat="1">
       <c r="A68" s="4" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="B68" s="7" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="D68" s="3"/>
       <c r="E68" s="4"/>
@@ -2953,13 +3011,13 @@
     </row>
     <row r="69" spans="1:11" s="2" customFormat="1">
       <c r="A69" s="4" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="B69" s="7" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
       <c r="D69" s="3"/>
       <c r="E69" s="4"/>
@@ -2972,13 +3030,13 @@
     </row>
     <row r="70" spans="1:11" s="2" customFormat="1">
       <c r="A70" s="4" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="B70" s="7" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="D70" s="3"/>
       <c r="E70" s="4"/>
@@ -2991,13 +3049,13 @@
     </row>
     <row r="71" spans="1:11" s="2" customFormat="1">
       <c r="A71" s="4" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="D71" s="3"/>
       <c r="E71" s="4"/>
@@ -3010,13 +3068,13 @@
     </row>
     <row r="72" spans="1:11" s="2" customFormat="1">
       <c r="A72" s="4" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>285</v>
+        <v>278</v>
       </c>
       <c r="D72" s="3"/>
       <c r="E72" s="4"/>
@@ -3029,13 +3087,13 @@
     </row>
     <row r="73" spans="1:11" s="2" customFormat="1">
       <c r="A73" s="4" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
       <c r="B73" s="7" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="D73" s="3"/>
       <c r="E73" s="4"/>
@@ -3048,13 +3106,13 @@
     </row>
     <row r="74" spans="1:11" s="2" customFormat="1">
       <c r="A74" s="4" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="B74" s="7" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
       <c r="D74" s="3"/>
       <c r="E74" s="4"/>
@@ -3067,13 +3125,13 @@
     </row>
     <row r="75" spans="1:11" s="2" customFormat="1">
       <c r="A75" s="4" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="B75" s="7" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>288</v>
+        <v>281</v>
       </c>
       <c r="D75" s="3"/>
       <c r="E75" s="4"/>
@@ -3086,13 +3144,13 @@
     </row>
     <row r="76" spans="1:11" s="2" customFormat="1">
       <c r="A76" s="4" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="B76" s="7" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>290</v>
+        <v>282</v>
       </c>
       <c r="D76" s="3"/>
       <c r="E76" s="4"/>
@@ -3105,13 +3163,13 @@
     </row>
     <row r="77" spans="1:11" s="2" customFormat="1">
       <c r="A77" s="4" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="B77" s="7" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
       <c r="D77" s="3"/>
       <c r="E77" s="4"/>
@@ -3124,13 +3182,13 @@
     </row>
     <row r="78" spans="1:11" s="2" customFormat="1">
       <c r="A78" s="4" t="s">
-        <v>293</v>
+        <v>254</v>
       </c>
       <c r="B78" s="7" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>292</v>
+        <v>285</v>
       </c>
       <c r="D78" s="3"/>
       <c r="E78" s="4"/>
@@ -3143,13 +3201,13 @@
     </row>
     <row r="79" spans="1:11" s="2" customFormat="1">
       <c r="A79" s="4" t="s">
-        <v>153</v>
+        <v>287</v>
       </c>
       <c r="B79" s="7" t="s">
-        <v>154</v>
+        <v>270</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>155</v>
+        <v>286</v>
       </c>
       <c r="D79" s="3"/>
       <c r="E79" s="4"/>
@@ -3162,13 +3220,13 @@
     </row>
     <row r="80" spans="1:11" s="2" customFormat="1">
       <c r="A80" s="4" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="B80" s="7" t="s">
-        <v>168</v>
+        <v>148</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="D80" s="3"/>
       <c r="E80" s="4"/>
@@ -3181,13 +3239,13 @@
     </row>
     <row r="81" spans="1:11" s="2" customFormat="1">
       <c r="A81" s="4" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="B81" s="7" t="s">
-        <v>64</v>
+        <v>162</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>81</v>
+        <v>151</v>
       </c>
       <c r="D81" s="3"/>
       <c r="E81" s="4"/>
@@ -3200,13 +3258,13 @@
     </row>
     <row r="82" spans="1:11" s="2" customFormat="1">
       <c r="A82" s="4" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="B82" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D82" s="3"/>
       <c r="E82" s="4"/>
@@ -3219,13 +3277,13 @@
     </row>
     <row r="83" spans="1:11" s="2" customFormat="1">
       <c r="A83" s="4" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="B83" s="7" t="s">
-        <v>165</v>
+        <v>65</v>
       </c>
       <c r="C83" s="4" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D83" s="3"/>
       <c r="E83" s="4"/>
@@ -3238,13 +3296,13 @@
     </row>
     <row r="84" spans="1:11" s="2" customFormat="1">
       <c r="A84" s="4" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="B84" s="7" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="D84" s="3"/>
       <c r="E84" s="4"/>
@@ -3257,13 +3315,13 @@
     </row>
     <row r="85" spans="1:11" s="2" customFormat="1">
       <c r="A85" s="4" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="B85" s="7" t="s">
-        <v>73</v>
+        <v>160</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="D85" s="3"/>
       <c r="E85" s="4"/>
@@ -3276,13 +3334,13 @@
     </row>
     <row r="86" spans="1:11" s="2" customFormat="1">
       <c r="A86" s="4" t="s">
-        <v>164</v>
-      </c>
-      <c r="B86" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
+      </c>
+      <c r="B86" s="7" t="s">
+        <v>73</v>
       </c>
       <c r="C86" s="4" t="s">
-        <v>158</v>
+        <v>88</v>
       </c>
       <c r="D86" s="3"/>
       <c r="E86" s="4"/>
@@ -3295,13 +3353,13 @@
     </row>
     <row r="87" spans="1:11" s="2" customFormat="1">
       <c r="A87" s="4" t="s">
-        <v>167</v>
-      </c>
-      <c r="B87" s="7" t="s">
-        <v>72</v>
+        <v>158</v>
+      </c>
+      <c r="B87" s="4" t="s">
+        <v>152</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>87</v>
+        <v>152</v>
       </c>
       <c r="D87" s="3"/>
       <c r="E87" s="4"/>
@@ -3314,13 +3372,13 @@
     </row>
     <row r="88" spans="1:11" s="2" customFormat="1">
       <c r="A88" s="4" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="B88" s="7" t="s">
-        <v>170</v>
+        <v>72</v>
       </c>
       <c r="C88" s="4" t="s">
-        <v>171</v>
+        <v>87</v>
       </c>
       <c r="D88" s="3"/>
       <c r="E88" s="4"/>
@@ -3333,13 +3391,13 @@
     </row>
     <row r="89" spans="1:11" s="2" customFormat="1">
       <c r="A89" s="4" t="s">
-        <v>174</v>
+        <v>163</v>
       </c>
       <c r="B89" s="7" t="s">
-        <v>175</v>
+        <v>164</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
       <c r="D89" s="3"/>
       <c r="E89" s="4"/>
@@ -3352,13 +3410,13 @@
     </row>
     <row r="90" spans="1:11" s="2" customFormat="1">
       <c r="A90" s="4" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="B90" s="7" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="C90" s="4" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="D90" s="3"/>
       <c r="E90" s="4"/>
@@ -3371,13 +3429,13 @@
     </row>
     <row r="91" spans="1:11" s="2" customFormat="1">
       <c r="A91" s="4" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="B91" s="7" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="C91" s="4" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="D91" s="3"/>
       <c r="E91" s="4"/>
@@ -3390,13 +3448,13 @@
     </row>
     <row r="92" spans="1:11" s="2" customFormat="1">
       <c r="A92" s="4" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="B92" s="7" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="C92" s="4" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="D92" s="3"/>
       <c r="E92" s="4"/>
@@ -3409,13 +3467,13 @@
     </row>
     <row r="93" spans="1:11" s="2" customFormat="1">
       <c r="A93" s="4" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="B93" s="7" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="C93" s="4" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="D93" s="3"/>
       <c r="E93" s="4"/>
@@ -3428,13 +3486,13 @@
     </row>
     <row r="94" spans="1:11" s="2" customFormat="1">
       <c r="A94" s="4" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="B94" s="7" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="C94" s="4" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="D94" s="3"/>
       <c r="E94" s="4"/>
@@ -3447,13 +3505,13 @@
     </row>
     <row r="95" spans="1:11" s="2" customFormat="1">
       <c r="A95" s="4" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="B95" s="7" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="C95" s="4" t="s">
-        <v>198</v>
+        <v>185</v>
       </c>
       <c r="D95" s="3"/>
       <c r="E95" s="4"/>
@@ -3466,13 +3524,13 @@
     </row>
     <row r="96" spans="1:11" s="2" customFormat="1">
       <c r="A96" s="4" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="B96" s="7" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="C96" s="4" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="D96" s="3"/>
       <c r="E96" s="4"/>
@@ -3485,13 +3543,13 @@
     </row>
     <row r="97" spans="1:11" s="2" customFormat="1">
       <c r="A97" s="4" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="B97" s="7" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="C97" s="4" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="D97" s="3"/>
       <c r="E97" s="4"/>
@@ -3504,13 +3562,13 @@
     </row>
     <row r="98" spans="1:11" s="2" customFormat="1">
       <c r="A98" s="4" t="s">
-        <v>201</v>
+        <v>188</v>
       </c>
       <c r="B98" s="7" t="s">
-        <v>202</v>
+        <v>191</v>
       </c>
       <c r="C98" s="4" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
       <c r="D98" s="3"/>
       <c r="E98" s="4"/>
@@ -3523,13 +3581,13 @@
     </row>
     <row r="99" spans="1:11" s="2" customFormat="1">
       <c r="A99" s="4" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="B99" s="7" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
       <c r="C99" s="4" t="s">
-        <v>208</v>
+        <v>197</v>
       </c>
       <c r="D99" s="3"/>
       <c r="E99" s="4"/>
@@ -3542,13 +3600,13 @@
     </row>
     <row r="100" spans="1:11" s="2" customFormat="1">
       <c r="A100" s="4" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="B100" s="7" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="C100" s="4" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="D100" s="3"/>
       <c r="E100" s="4"/>
@@ -3561,13 +3619,13 @@
     </row>
     <row r="101" spans="1:11" s="2" customFormat="1">
       <c r="A101" s="4" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
       <c r="B101" s="7" t="s">
-        <v>178</v>
+        <v>200</v>
       </c>
       <c r="C101" s="4" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="D101" s="3"/>
       <c r="E101" s="4"/>
@@ -3580,13 +3638,13 @@
     </row>
     <row r="102" spans="1:11" s="2" customFormat="1">
       <c r="A102" s="4" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="B102" s="7" t="s">
-        <v>213</v>
+        <v>172</v>
       </c>
       <c r="C102" s="4" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="D102" s="3"/>
       <c r="E102" s="4"/>
@@ -3599,13 +3657,13 @@
     </row>
     <row r="103" spans="1:11" s="2" customFormat="1">
       <c r="A103" s="4" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="B103" s="7" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
       <c r="C103" s="4" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
       <c r="D103" s="3"/>
       <c r="E103" s="4"/>
@@ -3618,13 +3676,13 @@
     </row>
     <row r="104" spans="1:11" s="2" customFormat="1">
       <c r="A104" s="4" t="s">
-        <v>219</v>
+        <v>209</v>
       </c>
       <c r="B104" s="7" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
       <c r="C104" s="4" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
       <c r="D104" s="3"/>
       <c r="E104" s="4"/>
@@ -3637,13 +3695,13 @@
     </row>
     <row r="105" spans="1:11" s="2" customFormat="1">
       <c r="A105" s="4" t="s">
-        <v>294</v>
+        <v>213</v>
       </c>
       <c r="B105" s="7" t="s">
-        <v>297</v>
+        <v>214</v>
       </c>
       <c r="C105" s="4" t="s">
-        <v>300</v>
+        <v>215</v>
       </c>
       <c r="D105" s="3"/>
       <c r="E105" s="4"/>
@@ -3656,13 +3714,13 @@
     </row>
     <row r="106" spans="1:11" s="2" customFormat="1">
       <c r="A106" s="4" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
       <c r="B106" s="7" t="s">
-        <v>299</v>
+        <v>291</v>
       </c>
       <c r="C106" s="4" t="s">
-        <v>301</v>
+        <v>294</v>
       </c>
       <c r="D106" s="3"/>
       <c r="E106" s="4"/>
@@ -3675,13 +3733,13 @@
     </row>
     <row r="107" spans="1:11" s="2" customFormat="1">
       <c r="A107" s="4" t="s">
-        <v>296</v>
+        <v>289</v>
       </c>
       <c r="B107" s="7" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="C107" s="4" t="s">
-        <v>302</v>
+        <v>295</v>
       </c>
       <c r="D107" s="3"/>
       <c r="E107" s="4"/>
@@ -3694,13 +3752,13 @@
     </row>
     <row r="108" spans="1:11" s="2" customFormat="1">
       <c r="A108" s="4" t="s">
-        <v>303</v>
+        <v>290</v>
       </c>
       <c r="B108" s="7" t="s">
-        <v>80</v>
+        <v>292</v>
       </c>
       <c r="C108" s="4" t="s">
-        <v>50</v>
+        <v>296</v>
       </c>
       <c r="D108" s="3"/>
       <c r="E108" s="4"/>
@@ -3713,13 +3771,13 @@
     </row>
     <row r="109" spans="1:11" s="2" customFormat="1">
       <c r="A109" s="4" t="s">
-        <v>304</v>
+        <v>297</v>
       </c>
       <c r="B109" s="7" t="s">
-        <v>308</v>
+        <v>80</v>
       </c>
       <c r="C109" s="4" t="s">
-        <v>312</v>
+        <v>50</v>
       </c>
       <c r="D109" s="3"/>
       <c r="E109" s="4"/>
@@ -3732,13 +3790,13 @@
     </row>
     <row r="110" spans="1:11" s="2" customFormat="1">
       <c r="A110" s="4" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="B110" s="7" t="s">
-        <v>309</v>
+        <v>302</v>
       </c>
       <c r="C110" s="4" t="s">
-        <v>313</v>
+        <v>306</v>
       </c>
       <c r="D110" s="3"/>
       <c r="E110" s="4"/>
@@ -3751,13 +3809,13 @@
     </row>
     <row r="111" spans="1:11" s="2" customFormat="1">
       <c r="A111" s="4" t="s">
-        <v>306</v>
+        <v>299</v>
       </c>
       <c r="B111" s="7" t="s">
-        <v>310</v>
+        <v>303</v>
       </c>
       <c r="C111" s="4" t="s">
-        <v>314</v>
+        <v>307</v>
       </c>
       <c r="D111" s="3"/>
       <c r="E111" s="4"/>
@@ -3770,13 +3828,13 @@
     </row>
     <row r="112" spans="1:11" s="2" customFormat="1">
       <c r="A112" s="4" t="s">
-        <v>307</v>
+        <v>300</v>
       </c>
       <c r="B112" s="7" t="s">
-        <v>311</v>
+        <v>304</v>
       </c>
       <c r="C112" s="4" t="s">
-        <v>315</v>
+        <v>308</v>
       </c>
       <c r="D112" s="3"/>
       <c r="E112" s="4"/>
@@ -3789,13 +3847,13 @@
     </row>
     <row r="113" spans="1:11" s="2" customFormat="1">
       <c r="A113" s="4" t="s">
-        <v>316</v>
+        <v>301</v>
       </c>
       <c r="B113" s="7" t="s">
-        <v>317</v>
+        <v>305</v>
       </c>
       <c r="C113" s="4" t="s">
-        <v>318</v>
+        <v>309</v>
       </c>
       <c r="D113" s="3"/>
       <c r="E113" s="4"/>
@@ -3808,13 +3866,13 @@
     </row>
     <row r="114" spans="1:11" s="2" customFormat="1">
       <c r="A114" s="4" t="s">
-        <v>319</v>
+        <v>310</v>
       </c>
       <c r="B114" s="7" t="s">
-        <v>321</v>
+        <v>311</v>
       </c>
       <c r="C114" s="4" t="s">
-        <v>323</v>
+        <v>312</v>
       </c>
       <c r="D114" s="3"/>
       <c r="E114" s="4"/>
@@ -3827,13 +3885,13 @@
     </row>
     <row r="115" spans="1:11" s="2" customFormat="1">
       <c r="A115" s="4" t="s">
-        <v>320</v>
+        <v>313</v>
       </c>
       <c r="B115" s="7" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
       <c r="C115" s="4" t="s">
-        <v>324</v>
+        <v>317</v>
       </c>
       <c r="D115" s="3"/>
       <c r="E115" s="4"/>
@@ -3846,13 +3904,13 @@
     </row>
     <row r="116" spans="1:11" s="2" customFormat="1">
       <c r="A116" s="4" t="s">
-        <v>325</v>
+        <v>314</v>
       </c>
       <c r="B116" s="7" t="s">
-        <v>326</v>
+        <v>316</v>
       </c>
       <c r="C116" s="4" t="s">
-        <v>327</v>
+        <v>318</v>
       </c>
       <c r="D116" s="3"/>
       <c r="E116" s="4"/>
@@ -3865,13 +3923,13 @@
     </row>
     <row r="117" spans="1:11" s="2" customFormat="1">
       <c r="A117" s="4" t="s">
-        <v>328</v>
+        <v>319</v>
       </c>
       <c r="B117" s="7" t="s">
-        <v>329</v>
+        <v>320</v>
       </c>
       <c r="C117" s="4" t="s">
-        <v>330</v>
+        <v>321</v>
       </c>
       <c r="D117" s="3"/>
       <c r="E117" s="4"/>
@@ -3884,13 +3942,13 @@
     </row>
     <row r="118" spans="1:11" s="2" customFormat="1">
       <c r="A118" s="4" t="s">
-        <v>331</v>
+        <v>322</v>
       </c>
       <c r="B118" s="7" t="s">
-        <v>332</v>
+        <v>323</v>
       </c>
       <c r="C118" s="4" t="s">
-        <v>333</v>
+        <v>324</v>
       </c>
       <c r="D118" s="3"/>
       <c r="E118" s="4"/>
@@ -3903,13 +3961,13 @@
     </row>
     <row r="119" spans="1:11" s="2" customFormat="1">
       <c r="A119" s="4" t="s">
-        <v>334</v>
+        <v>325</v>
       </c>
       <c r="B119" s="7" t="s">
-        <v>340</v>
+        <v>326</v>
       </c>
       <c r="C119" s="4" t="s">
-        <v>345</v>
+        <v>327</v>
       </c>
       <c r="D119" s="3"/>
       <c r="E119" s="4"/>
@@ -3922,13 +3980,13 @@
     </row>
     <row r="120" spans="1:11" s="2" customFormat="1">
       <c r="A120" s="4" t="s">
-        <v>335</v>
+        <v>328</v>
       </c>
       <c r="B120" s="7" t="s">
-        <v>341</v>
+        <v>334</v>
       </c>
       <c r="C120" s="4" t="s">
-        <v>346</v>
+        <v>339</v>
       </c>
       <c r="D120" s="3"/>
       <c r="E120" s="4"/>
@@ -3941,13 +3999,13 @@
     </row>
     <row r="121" spans="1:11" s="2" customFormat="1">
       <c r="A121" s="4" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B121" s="7" t="s">
-        <v>342</v>
+        <v>335</v>
       </c>
       <c r="C121" s="4" t="s">
-        <v>348</v>
+        <v>340</v>
       </c>
       <c r="D121" s="3"/>
       <c r="E121" s="4"/>
@@ -3960,13 +4018,13 @@
     </row>
     <row r="122" spans="1:11" s="2" customFormat="1">
       <c r="A122" s="4" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
       <c r="B122" s="7" t="s">
-        <v>343</v>
+        <v>336</v>
       </c>
       <c r="C122" s="4" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="D122" s="3"/>
       <c r="E122" s="4"/>
@@ -3979,13 +4037,13 @@
     </row>
     <row r="123" spans="1:11" s="2" customFormat="1">
       <c r="A123" s="4" t="s">
-        <v>339</v>
+        <v>332</v>
       </c>
       <c r="B123" s="7" t="s">
-        <v>344</v>
+        <v>337</v>
       </c>
       <c r="C123" s="4" t="s">
-        <v>349</v>
+        <v>341</v>
       </c>
       <c r="D123" s="3"/>
       <c r="E123" s="4"/>
@@ -3998,13 +4056,13 @@
     </row>
     <row r="124" spans="1:11" s="2" customFormat="1">
       <c r="A124" s="4" t="s">
-        <v>350</v>
+        <v>333</v>
       </c>
       <c r="B124" s="7" t="s">
-        <v>358</v>
+        <v>338</v>
       </c>
       <c r="C124" s="4" t="s">
-        <v>366</v>
+        <v>343</v>
       </c>
       <c r="D124" s="3"/>
       <c r="E124" s="4"/>
@@ -4017,13 +4075,13 @@
     </row>
     <row r="125" spans="1:11" s="2" customFormat="1">
       <c r="A125" s="4" t="s">
-        <v>351</v>
+        <v>344</v>
       </c>
       <c r="B125" s="7" t="s">
-        <v>359</v>
+        <v>352</v>
       </c>
       <c r="C125" s="4" t="s">
-        <v>367</v>
+        <v>360</v>
       </c>
       <c r="D125" s="3"/>
       <c r="E125" s="4"/>
@@ -4036,13 +4094,13 @@
     </row>
     <row r="126" spans="1:11" s="2" customFormat="1">
       <c r="A126" s="4" t="s">
-        <v>352</v>
+        <v>345</v>
       </c>
       <c r="B126" s="7" t="s">
-        <v>360</v>
+        <v>353</v>
       </c>
       <c r="C126" s="4" t="s">
-        <v>370</v>
+        <v>361</v>
       </c>
       <c r="D126" s="3"/>
       <c r="E126" s="4"/>
@@ -4055,13 +4113,13 @@
     </row>
     <row r="127" spans="1:11" s="2" customFormat="1">
       <c r="A127" s="4" t="s">
-        <v>353</v>
+        <v>346</v>
       </c>
       <c r="B127" s="7" t="s">
-        <v>361</v>
+        <v>354</v>
       </c>
       <c r="C127" s="4" t="s">
-        <v>371</v>
+        <v>364</v>
       </c>
       <c r="D127" s="3"/>
       <c r="E127" s="4"/>
@@ -4074,13 +4132,13 @@
     </row>
     <row r="128" spans="1:11" s="2" customFormat="1">
       <c r="A128" s="4" t="s">
-        <v>354</v>
+        <v>347</v>
       </c>
       <c r="B128" s="7" t="s">
-        <v>362</v>
+        <v>355</v>
       </c>
       <c r="C128" s="4" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="D128" s="3"/>
       <c r="E128" s="4"/>
@@ -4093,13 +4151,13 @@
     </row>
     <row r="129" spans="1:11" s="2" customFormat="1">
       <c r="A129" s="4" t="s">
-        <v>355</v>
+        <v>348</v>
       </c>
       <c r="B129" s="7" t="s">
-        <v>363</v>
+        <v>356</v>
       </c>
       <c r="C129" s="4" t="s">
-        <v>369</v>
+        <v>362</v>
       </c>
       <c r="D129" s="3"/>
       <c r="E129" s="4"/>
@@ -4112,13 +4170,13 @@
     </row>
     <row r="130" spans="1:11" s="2" customFormat="1">
       <c r="A130" s="4" t="s">
-        <v>356</v>
+        <v>349</v>
       </c>
       <c r="B130" s="7" t="s">
-        <v>364</v>
+        <v>357</v>
       </c>
       <c r="C130" s="4" t="s">
-        <v>372</v>
+        <v>363</v>
       </c>
       <c r="D130" s="3"/>
       <c r="E130" s="4"/>
@@ -4131,13 +4189,13 @@
     </row>
     <row r="131" spans="1:11" s="2" customFormat="1">
       <c r="A131" s="4" t="s">
-        <v>357</v>
+        <v>350</v>
       </c>
       <c r="B131" s="7" t="s">
-        <v>365</v>
+        <v>358</v>
       </c>
       <c r="C131" s="4" t="s">
-        <v>373</v>
+        <v>366</v>
       </c>
       <c r="D131" s="3"/>
       <c r="E131" s="4"/>
@@ -4150,13 +4208,13 @@
     </row>
     <row r="132" spans="1:11" s="2" customFormat="1">
       <c r="A132" s="4" t="s">
-        <v>374</v>
+        <v>351</v>
       </c>
       <c r="B132" s="7" t="s">
-        <v>375</v>
+        <v>359</v>
       </c>
       <c r="C132" s="4" t="s">
-        <v>376</v>
+        <v>367</v>
       </c>
       <c r="D132" s="3"/>
       <c r="E132" s="4"/>
@@ -4169,13 +4227,13 @@
     </row>
     <row r="133" spans="1:11" s="2" customFormat="1">
       <c r="A133" s="4" t="s">
-        <v>377</v>
+        <v>368</v>
       </c>
       <c r="B133" s="7" t="s">
-        <v>378</v>
+        <v>369</v>
       </c>
       <c r="C133" s="4" t="s">
-        <v>379</v>
+        <v>370</v>
       </c>
       <c r="D133" s="3"/>
       <c r="E133" s="4"/>
@@ -4188,13 +4246,13 @@
     </row>
     <row r="134" spans="1:11" s="2" customFormat="1">
       <c r="A134" s="4" t="s">
-        <v>380</v>
+        <v>371</v>
       </c>
       <c r="B134" s="7" t="s">
-        <v>381</v>
+        <v>372</v>
       </c>
       <c r="C134" s="4" t="s">
-        <v>382</v>
+        <v>373</v>
       </c>
       <c r="D134" s="3"/>
       <c r="E134" s="4"/>
@@ -4206,9 +4264,15 @@
       <c r="K134" s="11"/>
     </row>
     <row r="135" spans="1:11" s="2" customFormat="1">
-      <c r="A135" s="4"/>
-      <c r="B135" s="7"/>
-      <c r="C135" s="4"/>
+      <c r="A135" s="4" t="s">
+        <v>374</v>
+      </c>
+      <c r="B135" s="7" t="s">
+        <v>375</v>
+      </c>
+      <c r="C135" s="4" t="s">
+        <v>376</v>
+      </c>
       <c r="D135" s="3"/>
       <c r="E135" s="4"/>
       <c r="F135" s="4"/>
@@ -4219,9 +4283,15 @@
       <c r="K135" s="11"/>
     </row>
     <row r="136" spans="1:11" s="2" customFormat="1">
-      <c r="A136" s="4"/>
-      <c r="B136" s="7"/>
-      <c r="C136" s="4"/>
+      <c r="A136" s="4" t="s">
+        <v>377</v>
+      </c>
+      <c r="B136" s="7" t="s">
+        <v>393</v>
+      </c>
+      <c r="C136" s="4" t="s">
+        <v>378</v>
+      </c>
       <c r="D136" s="3"/>
       <c r="E136" s="4"/>
       <c r="F136" s="4"/>
@@ -4232,9 +4302,15 @@
       <c r="K136" s="11"/>
     </row>
     <row r="137" spans="1:11" s="2" customFormat="1">
-      <c r="A137" s="4"/>
-      <c r="B137" s="7"/>
-      <c r="C137" s="4"/>
+      <c r="A137" s="4" t="s">
+        <v>379</v>
+      </c>
+      <c r="B137" s="7" t="s">
+        <v>380</v>
+      </c>
+      <c r="C137" s="4" t="s">
+        <v>380</v>
+      </c>
       <c r="D137" s="3"/>
       <c r="E137" s="4"/>
       <c r="F137" s="4"/>
@@ -4245,9 +4321,15 @@
       <c r="K137" s="11"/>
     </row>
     <row r="138" spans="1:11" s="2" customFormat="1">
-      <c r="A138" s="4"/>
-      <c r="B138" s="7"/>
-      <c r="C138" s="4"/>
+      <c r="A138" s="4" t="s">
+        <v>381</v>
+      </c>
+      <c r="B138" s="7" t="s">
+        <v>382</v>
+      </c>
+      <c r="C138" s="4" t="s">
+        <v>383</v>
+      </c>
       <c r="D138" s="3"/>
       <c r="E138" s="4"/>
       <c r="F138" s="4"/>
@@ -4258,9 +4340,15 @@
       <c r="K138" s="11"/>
     </row>
     <row r="139" spans="1:11" s="2" customFormat="1">
-      <c r="A139" s="4"/>
-      <c r="B139" s="7"/>
-      <c r="C139" s="4"/>
+      <c r="A139" s="4" t="s">
+        <v>384</v>
+      </c>
+      <c r="B139" s="7" t="s">
+        <v>385</v>
+      </c>
+      <c r="C139" s="4" t="s">
+        <v>386</v>
+      </c>
       <c r="D139" s="3"/>
       <c r="E139" s="4"/>
       <c r="F139" s="4"/>
@@ -4271,9 +4359,15 @@
       <c r="K139" s="11"/>
     </row>
     <row r="140" spans="1:11" s="2" customFormat="1">
-      <c r="A140" s="4"/>
-      <c r="B140" s="7"/>
-      <c r="C140" s="4"/>
+      <c r="A140" s="4" t="s">
+        <v>387</v>
+      </c>
+      <c r="B140" s="7" t="s">
+        <v>388</v>
+      </c>
+      <c r="C140" s="4" t="s">
+        <v>389</v>
+      </c>
       <c r="D140" s="3"/>
       <c r="E140" s="4"/>
       <c r="F140" s="4"/>
@@ -4284,9 +4378,15 @@
       <c r="K140" s="11"/>
     </row>
     <row r="141" spans="1:11" s="2" customFormat="1">
-      <c r="A141" s="4"/>
-      <c r="B141" s="7"/>
-      <c r="C141" s="4"/>
+      <c r="A141" s="4" t="s">
+        <v>394</v>
+      </c>
+      <c r="B141" s="7" t="s">
+        <v>395</v>
+      </c>
+      <c r="C141" s="4" t="s">
+        <v>396</v>
+      </c>
       <c r="D141" s="3"/>
       <c r="E141" s="4"/>
       <c r="F141" s="4"/>
@@ -4297,9 +4397,15 @@
       <c r="K141" s="11"/>
     </row>
     <row r="142" spans="1:11" s="2" customFormat="1">
-      <c r="A142" s="4"/>
-      <c r="B142" s="7"/>
-      <c r="C142" s="4"/>
+      <c r="A142" s="4" t="s">
+        <v>390</v>
+      </c>
+      <c r="B142" s="7" t="s">
+        <v>391</v>
+      </c>
+      <c r="C142" s="4" t="s">
+        <v>392</v>
+      </c>
       <c r="D142" s="3"/>
       <c r="E142" s="4"/>
       <c r="F142" s="4"/>
@@ -4309,10 +4415,16 @@
       <c r="J142" s="10"/>
       <c r="K142" s="11"/>
     </row>
-    <row r="143" spans="1:11" s="2" customFormat="1">
-      <c r="A143" s="4"/>
-      <c r="B143" s="7"/>
-      <c r="C143" s="4"/>
+    <row r="143" spans="1:11" s="2" customFormat="1" ht="28.5">
+      <c r="A143" s="4" t="s">
+        <v>398</v>
+      </c>
+      <c r="B143" s="7" t="s">
+        <v>399</v>
+      </c>
+      <c r="C143" s="4" t="s">
+        <v>400</v>
+      </c>
       <c r="D143" s="3"/>
       <c r="E143" s="4"/>
       <c r="F143" s="4"/>
@@ -4323,9 +4435,15 @@
       <c r="K143" s="11"/>
     </row>
     <row r="144" spans="1:11" s="2" customFormat="1">
-      <c r="A144" s="4"/>
-      <c r="B144" s="7"/>
-      <c r="C144" s="4"/>
+      <c r="A144" s="4" t="s">
+        <v>325</v>
+      </c>
+      <c r="B144" s="7" t="s">
+        <v>401</v>
+      </c>
+      <c r="C144" s="4" t="s">
+        <v>327</v>
+      </c>
       <c r="D144" s="3"/>
       <c r="E144" s="4"/>
       <c r="F144" s="4"/>
@@ -16698,10 +16816,18 @@
       <c r="J1095" s="10"/>
       <c r="K1095" s="11"/>
     </row>
-    <row r="1096" spans="1:11">
-      <c r="A1096" s="8"/>
-      <c r="B1096" s="8"/>
-      <c r="C1096" s="8"/>
+    <row r="1096" spans="1:11" s="2" customFormat="1">
+      <c r="A1096" s="4"/>
+      <c r="B1096" s="7"/>
+      <c r="C1096" s="4"/>
+      <c r="D1096" s="3"/>
+      <c r="E1096" s="4"/>
+      <c r="F1096" s="4"/>
+      <c r="G1096" s="4"/>
+      <c r="H1096" s="4"/>
+      <c r="I1096" s="4"/>
+      <c r="J1096" s="10"/>
+      <c r="K1096" s="11"/>
     </row>
     <row r="1097" spans="1:11">
       <c r="A1097" s="8"/>
@@ -16718,8 +16844,13 @@
       <c r="B1099" s="8"/>
       <c r="C1099" s="8"/>
     </row>
+    <row r="1100" spans="1:11">
+      <c r="A1100" s="8"/>
+      <c r="B1100" s="8"/>
+      <c r="C1100" s="8"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:I690" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:I691" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>